<commit_message>
Found object signature issue
</commit_message>
<xml_diff>
--- a/output-refactored.xlsx
+++ b/output-refactored.xlsx
@@ -397,127 +397,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>incidentId</v>
+        <v>employeeId</v>
       </c>
       <c r="B1" t="str">
-        <v>type</v>
+        <v>firstName</v>
       </c>
       <c r="C1" t="str">
-        <v>time</v>
+        <v>personalInfo.dateOfBirth</v>
       </c>
       <c r="D1" t="str">
-        <v>status</v>
+        <v>personalInfo.phoneNumber</v>
       </c>
       <c r="E1" t="str">
-        <v>location.road</v>
+        <v>personalInfo.emergencyContact</v>
       </c>
       <c r="F1" t="str">
-        <v>location.direction</v>
+        <v>lastName</v>
       </c>
       <c r="G1" t="str">
-        <v>location.landmark</v>
+        <v>email</v>
       </c>
       <c r="H1" t="str">
-        <v>details.vehiclesInvolved.type</v>
+        <v>performanceReviews.reviewId</v>
       </c>
       <c r="I1" t="str">
-        <v>details.vehiclesInvolved.plateNumber.serial</v>
+        <v>performanceReviews.reviewDate</v>
       </c>
       <c r="J1" t="str">
-        <v>details.vehiclesInvolved.plateNumber.region</v>
+        <v>performanceReviews.metrics.metricName</v>
       </c>
       <c r="K1" t="str">
-        <v>details.vehiclesInvolved.severity</v>
+        <v>performanceReviews.metrics.scores</v>
       </c>
       <c r="L1" t="str">
-        <v>details.casualties</v>
+        <v>skills.skillName</v>
       </c>
       <c r="M1" t="str">
-        <v>details.lanesBlocked</v>
+        <v>skills.proficiencyLevel</v>
       </c>
       <c r="N1" t="str">
-        <v>advisories.type</v>
+        <v>trainingHistory.courseName</v>
       </c>
       <c r="O1" t="str">
-        <v>advisories.message</v>
+        <v>trainingHistory.completionDate</v>
       </c>
       <c r="P1" t="str">
-        <v>responders.agency</v>
+        <v>trainingHistory.certifications.certificationName</v>
       </c>
       <c r="Q1" t="str">
-        <v>responders.arrivalTime</v>
-      </c>
-      <c r="R1" t="str">
-        <v>responders.personnel.name</v>
-      </c>
-      <c r="S1" t="str">
-        <v>responders.personnel.role</v>
+        <v>trainingHistory.certifications.issueDate</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>INC001</v>
+        <v>EMP-2024-001</v>
       </c>
       <c r="B2" t="str">
-        <v>Accident</v>
+        <v>Sarah</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-05-17T07:35:00+08:00</v>
+        <v>1990-03-15</v>
       </c>
       <c r="D2" t="str">
-        <v>Ongoing</v>
+        <v>+1-555-0123</v>
       </c>
       <c r="E2" t="str">
-        <v>PIE</v>
+        <v>John Mitchell (Spouse)</v>
       </c>
       <c r="F2" t="str">
-        <v>towards Tuas</v>
+        <v>Johnson</v>
       </c>
       <c r="G2" t="str">
-        <v>before Eunos Exit</v>
+        <v>sarah.johnson@company.com</v>
       </c>
       <c r="H2" t="str">
-        <v>Car</v>
+        <v>REV-2024-Q1</v>
       </c>
       <c r="I2" t="str">
-        <v>SBC1234X</v>
+        <v>2024-03-15</v>
       </c>
       <c r="J2" t="str">
-        <v>SG</v>
-      </c>
-      <c r="K2" t="str">
-        <v>Moderate</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
+        <v>Communication 1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" t="str">
+        <v>JavaScript</v>
       </c>
       <c r="M2" t="str">
-        <v>Lane 1, Lane 2</v>
+        <v>Expert</v>
       </c>
       <c r="N2" t="str">
-        <v>Diversion</v>
+        <v>Advanced Leadership Development</v>
       </c>
       <c r="O2" t="str">
-        <v>Use Exit 10A to Eunos Link</v>
+        <v>2024-02-28</v>
       </c>
       <c r="P2" t="str">
-        <v>Traffic Police</v>
+        <v>Certified Scrum Master</v>
       </c>
       <c r="Q2" t="str">
-        <v>2025-05-17T07:45:00+08:00</v>
-      </c>
-      <c r="R2" t="str">
-        <v>Sgt. Tan Wei</v>
-      </c>
-      <c r="S2" t="str">
-        <v>Team Leader</v>
+        <v>2024-01-15</v>
       </c>
     </row>
     <row r="3">
@@ -543,40 +531,34 @@
         <v/>
       </c>
       <c r="H3" t="str">
-        <v>Motorcycle</v>
+        <v/>
       </c>
       <c r="I3" t="str">
-        <v>SBC2334X</v>
+        <v/>
       </c>
       <c r="J3" t="str">
-        <v>ML</v>
-      </c>
-      <c r="K3" t="str">
-        <v>High</v>
+        <v>Communication 2</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>Project Management</v>
       </c>
       <c r="M3" t="str">
-        <v/>
+        <v>Intermediate</v>
       </c>
       <c r="N3" t="str">
-        <v>Congestion Alert</v>
+        <v/>
       </c>
       <c r="O3" t="str">
-        <v>Expect delays of up to 25 minutes</v>
+        <v/>
       </c>
       <c r="P3" t="str">
-        <v/>
+        <v>AWS Solutions Architect</v>
       </c>
       <c r="Q3" t="str">
-        <v/>
-      </c>
-      <c r="R3" t="str">
-        <v>Cpl. Lim Hui</v>
-      </c>
-      <c r="S3" t="str">
-        <v>Traffic Control</v>
+        <v>2023-11-20</v>
       </c>
     </row>
     <row r="4">
@@ -602,16 +584,16 @@
         <v/>
       </c>
       <c r="H4" t="str">
-        <v/>
+        <v>REV-2024-Q2</v>
       </c>
       <c r="I4" t="str">
-        <v/>
+        <v>2024-03-15</v>
       </c>
       <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
+        <v>Communication 3</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -626,16 +608,10 @@
         <v/>
       </c>
       <c r="P4" t="str">
-        <v>SCDF</v>
+        <v/>
       </c>
       <c r="Q4" t="str">
-        <v>2025-05-17T07:50:00+08:00</v>
-      </c>
-      <c r="R4" t="str">
-        <v>Lt. Ravi Kumar</v>
-      </c>
-      <c r="S4" t="str">
-        <v>Rescue Operations</v>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -667,10 +643,10 @@
         <v/>
       </c>
       <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
+        <v>Communication 4</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -689,71 +665,59 @@
       </c>
       <c r="Q5" t="str">
         <v/>
-      </c>
-      <c r="R5" t="str">
-        <v>Spec. Ong Jia</v>
-      </c>
-      <c r="S5" t="str">
-        <v>Rescue Operations</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>INC002</v>
+        <v>EMP-2024-002</v>
       </c>
       <c r="B6" t="str">
-        <v>Accident</v>
+        <v>Michael</v>
       </c>
       <c r="C6" t="str">
-        <v>2025-05-17T07:35:00+08:00</v>
+        <v>1985-07-22</v>
       </c>
       <c r="D6" t="str">
-        <v>Ongoing</v>
+        <v>+1-555-0456</v>
       </c>
       <c r="E6" t="str">
-        <v>AYE</v>
+        <v>Lisa Chen (Sister)</v>
       </c>
       <c r="F6" t="str">
-        <v>towards Tuas</v>
+        <v>Rodriguez</v>
       </c>
       <c r="G6" t="str">
-        <v>before Eunos Exit</v>
+        <v>michael.rodriguez@company.com</v>
       </c>
       <c r="H6" t="str">
-        <v>Truck</v>
+        <v>REV-2024-Q1-002</v>
       </c>
       <c r="I6" t="str">
-        <v>SBC1234X</v>
+        <v>2024-03-20</v>
       </c>
       <c r="J6" t="str">
-        <v>SG</v>
-      </c>
-      <c r="K6" t="str">
-        <v>Moderate</v>
-      </c>
-      <c r="L6">
+        <v>Technical Skills 1</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
+      <c r="L6" t="str">
+        <v>Employee Relations</v>
+      </c>
       <c r="M6" t="str">
-        <v>Lane 1, Lane 2</v>
+        <v>Expert</v>
       </c>
       <c r="N6" t="str">
-        <v>Diversion</v>
+        <v>Diversity and Inclusion Workshop</v>
       </c>
       <c r="O6" t="str">
-        <v>Use Exit 10A to Eunos Link</v>
+        <v>2024-01-10</v>
       </c>
       <c r="P6" t="str">
-        <v>SCDF</v>
+        <v>PHR Certification</v>
       </c>
       <c r="Q6" t="str">
-        <v>2025-05-17T07:45:00+08:00</v>
-      </c>
-      <c r="R6" t="str">
-        <v>Sgt. Tan Wei 2</v>
-      </c>
-      <c r="S6" t="str">
-        <v>Rescue Operations</v>
+        <v>2023-08-15</v>
       </c>
     </row>
     <row r="7">
@@ -779,163 +743,39 @@
         <v/>
       </c>
       <c r="H7" t="str">
-        <v>Motorcycle</v>
+        <v>REV-2024-Q1-003</v>
       </c>
       <c r="I7" t="str">
-        <v>SBC2334X</v>
+        <v>2024-03-20</v>
       </c>
       <c r="J7" t="str">
-        <v>ML</v>
-      </c>
-      <c r="K7" t="str">
-        <v>High</v>
+        <v>Technical Skills 2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
       </c>
       <c r="L7" t="str">
-        <v/>
+        <v>Data Analysis</v>
       </c>
       <c r="M7" t="str">
-        <v/>
+        <v>Intermediate</v>
       </c>
       <c r="N7" t="str">
-        <v>Congestion Alert</v>
+        <v/>
       </c>
       <c r="O7" t="str">
-        <v>Expect delays of up to 25 minutes</v>
+        <v/>
       </c>
       <c r="P7" t="str">
         <v/>
       </c>
       <c r="Q7" t="str">
         <v/>
-      </c>
-      <c r="R7" t="str">
-        <v>Cpl. Lim Hui 2</v>
-      </c>
-      <c r="S7" t="str">
-        <v>Rescue Operations</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v/>
-      </c>
-      <c r="B8" t="str">
-        <v/>
-      </c>
-      <c r="C8" t="str">
-        <v/>
-      </c>
-      <c r="D8" t="str">
-        <v/>
-      </c>
-      <c r="E8" t="str">
-        <v/>
-      </c>
-      <c r="F8" t="str">
-        <v/>
-      </c>
-      <c r="G8" t="str">
-        <v/>
-      </c>
-      <c r="H8" t="str">
-        <v/>
-      </c>
-      <c r="I8" t="str">
-        <v/>
-      </c>
-      <c r="J8" t="str">
-        <v/>
-      </c>
-      <c r="K8" t="str">
-        <v/>
-      </c>
-      <c r="L8" t="str">
-        <v/>
-      </c>
-      <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
-        <v/>
-      </c>
-      <c r="O8" t="str">
-        <v/>
-      </c>
-      <c r="P8" t="str">
-        <v>Traffic Police</v>
-      </c>
-      <c r="Q8" t="str">
-        <v>2025-05-17T07:50:00+08:00</v>
-      </c>
-      <c r="R8" t="str">
-        <v>Lt. Ravi Kumar 2</v>
-      </c>
-      <c r="S8" t="str">
-        <v>Rescue Operations</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v/>
-      </c>
-      <c r="B9" t="str">
-        <v/>
-      </c>
-      <c r="C9" t="str">
-        <v/>
-      </c>
-      <c r="D9" t="str">
-        <v/>
-      </c>
-      <c r="E9" t="str">
-        <v/>
-      </c>
-      <c r="F9" t="str">
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <v/>
-      </c>
-      <c r="H9" t="str">
-        <v/>
-      </c>
-      <c r="I9" t="str">
-        <v/>
-      </c>
-      <c r="J9" t="str">
-        <v/>
-      </c>
-      <c r="K9" t="str">
-        <v/>
-      </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-      <c r="M9" t="str">
-        <v/>
-      </c>
-      <c r="N9" t="str">
-        <v/>
-      </c>
-      <c r="O9" t="str">
-        <v/>
-      </c>
-      <c r="P9" t="str">
-        <v/>
-      </c>
-      <c r="Q9" t="str">
-        <v/>
-      </c>
-      <c r="R9" t="str">
-        <v>Spec. Ong Jia 2</v>
-      </c>
-      <c r="S9" t="str">
-        <v>Rescue Operations</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>